<commit_message>
Changed Open Application so it works both pre and post Version 2021
</commit_message>
<xml_diff>
--- a/Book Flights/Reusable/Default.xlsx
+++ b/Book Flights/Reusable/Default.xlsx
@@ -484,7 +484,7 @@
     <col min="1" max="16384" width="9.1484375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="12.75" customHeight="1" customFormat="1"/>
+    <row r="1" ht="12.75" customHeight="1" customFormat="1"/>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -508,7 +508,7 @@
     <col min="1" max="16384" width="9.1484375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="12.75" customHeight="1" customFormat="1"/>
+    <row r="1" ht="12.75" customHeight="1" customFormat="1"/>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -532,7 +532,7 @@
     <col min="1" max="16384" width="9.1484375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="12.75" customHeight="1" customFormat="1"/>
+    <row r="1" ht="12.75" customHeight="1" customFormat="1"/>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>